<commit_message>
[TDP-1481] finish serializer using event handler so not anymore whole document loaded in memory for serializing
Signed-off-by: olivier lamy <olamy@apache.org>
</commit_message>
<xml_diff>
--- a/dataprep-backend-common/src/test/resources/org/talend/dataprep/schema/xls/bad_formulas.xlsx
+++ b/dataprep-backend-common/src/test/resources/org/talend/dataprep/schema/xls/bad_formulas.xlsx
@@ -98,23 +98,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sumary"/>
       <sheetName val="Leads"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="D2" t="str">
-            <v>John</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3" t="str">
-            <v>John</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -445,12 +432,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -465,18 +452,18 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="str">
+      <c r="B2" s="1" t="e">
         <f>[1]Leads!$D$2</f>
-        <v>John</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" t="e">
         <f>[1]Leads!$D$3</f>
-        <v>John</v>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>